<commit_message>
added stories that have been fully completed in sprint 3
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siddharthajuluru/Documents/College/Spring-23/SWEN 261/team-project-2225-swen-261-04-d-sica/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE83E91E-33AC-A644-B2BC-DD435C10AB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110ED754-E5AB-7C4A-A158-C59BC205D29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Instructions</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>AK; 03/15/23</t>
+  </si>
+  <si>
+    <t>As a customer I want to be able to see the description so that I can know if the keyboard is something I would like to invest in.</t>
+  </si>
+  <si>
+    <t>**Given** I am an admin **when** create a product **then** I should be able to add a description at the time of creation.</t>
+  </si>
+  <si>
+    <t>**Given** I am a customer **when** I request a product **then** I should be able to see the product description.</t>
+  </si>
+  <si>
+    <t>SJ; 04/04/23</t>
   </si>
 </sst>
 </file>
@@ -637,7 +649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -685,9 +697,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F587"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D13" sqref="D13"/>
+      <selection pane="topRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -922,7 +934,7 @@
       </c>
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
@@ -934,7 +946,7 @@
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
         <v>32</v>
@@ -947,59 +959,79 @@
       </c>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C21" s="8"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" s="8"/>
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C23" s="8"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C24" s="8"/>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C25" s="8"/>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" s="8"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C27" s="8"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C28" s="8"/>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" s="8"/>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" s="8"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C31" s="8"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C32" s="8"/>
       <c r="E32" s="8"/>
     </row>
@@ -3233,7 +3265,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F587 D2:D587">
+  <conditionalFormatting sqref="D2:D587 F2:F587">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>

</xml_diff>

<commit_message>
acceptance test plan change
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siddharthajuluru/Documents/College/Spring-23/SWEN 261/team-project-2225-swen-261-04-d-sica/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D21FE4B-DCFE-8D45-830A-8416A4FD4928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D60DD7F-6542-F041-A677-8F55DFF50279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t>Instructions</t>
   </si>
@@ -174,24 +174,12 @@
     <t>As a customer I want to pick out my keyboard size so that I can build my desired keyboard.</t>
   </si>
   <si>
-    <t>**Given** I am a customer who wants a specific keyboard size **when** I enter the keyboard page **then** I expect to see all the different keyboard sizes and be able to sort keyboards based on size.</t>
-  </si>
-  <si>
     <t>As a customer I want to pick out my switches so that I can build my desired keyboard.</t>
   </si>
   <si>
-    <t>**Given** I am a customer who wants a specific switch **when** I enter the switch page **then** I expect to see all the different switches and be able to add them to my shopping cart.</t>
-  </si>
-  <si>
     <t>As a customer I want to pick out my keycaps so that I can build my desired keyboard.</t>
   </si>
   <si>
-    <t>**Given** I am a customer who wants a specific keycap **when** I enter the keycap page **then** I expect to see all the keycaps I can choose from and be able to add them to my shopping cart.</t>
-  </si>
-  <si>
-    <t>**Given** I am a customer who wants a specific keyboard case **when** I click on the case options **then** I expect to see all the different keyboard cases and the ability to add them to cart.</t>
-  </si>
-  <si>
     <t>As a customer I want to pick out my keyboard case so that I can build my desired keyboard.</t>
   </si>
   <si>
@@ -199,6 +187,27 @@
   </si>
   <si>
     <t>**Given** that I am a customer who wants a keyboard **when** I choose the option for a custom keyboard **then** I expect to be able to customize a keyboard.</t>
+  </si>
+  <si>
+    <t>**Given** I am a customer who wants a specific keyboard size **when** I enter the keyboard customizer page **then** I expect to be able to choose the keyboard size I want.</t>
+  </si>
+  <si>
+    <t>**Given** I am a customer who wants a specific switch **when** I enter the keyboard customizer page **then** I expect to see all the different switches and be able to be chosen</t>
+  </si>
+  <si>
+    <t>**Given** I am a customer who wants a specific keycap **when** I enter the keyboard customizer page **then** I expect to be able to change the way the keycaps look on my keyboard</t>
+  </si>
+  <si>
+    <t>**Given** I am a customer who wants a specific keyboard case **when** I click on the keyboard customizer page **then** I expect to be able to change the look of my keyboard case</t>
+  </si>
+  <si>
+    <t>CL; 04/08/23</t>
+  </si>
+  <si>
+    <t>IK; 04/08/23</t>
+  </si>
+  <si>
+    <t>SJ; 04/09/23</t>
   </si>
   <si>
     <r>
@@ -208,6 +217,7 @@
     <r>
       <rPr>
         <b/>
+        <strike/>
         <sz val="20"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
@@ -217,6 +227,7 @@
     <r>
       <rPr>
         <b/>
+        <strike/>
         <sz val="20"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -228,6 +239,7 @@
     <r>
       <rPr>
         <b/>
+        <strike/>
         <sz val="20"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
@@ -237,6 +249,7 @@
     <r>
       <rPr>
         <b/>
+        <strike/>
         <sz val="20"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -288,6 +301,7 @@
     </font>
     <font>
       <b/>
+      <strike/>
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -296,6 +310,7 @@
     </font>
     <font>
       <b/>
+      <strike/>
       <sz val="20"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
@@ -769,7 +784,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -804,7 +819,7 @@
     </row>
     <row r="6" spans="1:2" ht="108" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -821,9 +836,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F587"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="125" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A30" sqref="A30:B36"/>
+      <selection pane="topRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1119,14 +1134,24 @@
         <v>43</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
@@ -1134,57 +1159,87 @@
         <v>45</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="E23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" s="8"/>
@@ -3424,7 +3479,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="E2:E587 C2:C587">
+  <conditionalFormatting sqref="C2:C587 E2:E587">
     <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>

</xml_diff>